<commit_message>
queries for other questions
</commit_message>
<xml_diff>
--- a/tarea1/modelo/Facts Table.xlsx
+++ b/tarea1/modelo/Facts Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tarea1\Src\tarea1\modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FEDF5D-F246-40E8-81E7-A5163CC297AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F1B4A-E607-4082-9F22-994242B7C205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-13360" windowWidth="21820" windowHeight="38020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11565" yWindow="3870" windowWidth="18915" windowHeight="12885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Index" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>FACT GROUP NAME</t>
   </si>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
@@ -504,7 +506,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8898FBFD-4504-4516-A0A7-96C2B1D0493D}">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>